<commit_message>
Add new enumeration types
</commit_message>
<xml_diff>
--- a/nbs/files/lut/dbo_counmet.xlsx
+++ b/nbs/files/lut/dbo_counmet.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27103"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DC4F866-7A2D-4DF6-AF59-204F03AD030D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franckalbinet/pro/IAEA/MARIS/marisco/nbs/files/lut/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DE5C7D-0CA5-7942-B086-2ED0A94BE24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="23895" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="23900" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dbo_counmet" sheetId="1" r:id="rId1"/>
@@ -275,11 +280,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -324,9 +329,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -364,9 +369,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -399,9 +404,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -434,9 +456,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -613,16 +652,16 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="58.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="58.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -633,7 +672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -644,7 +683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -655,7 +694,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -666,7 +705,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -677,7 +716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -688,7 +727,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -699,7 +738,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -710,7 +749,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -721,7 +760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -732,7 +771,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -743,7 +782,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -754,7 +793,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -765,7 +804,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -776,7 +815,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -787,7 +826,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -798,7 +837,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -809,7 +848,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -820,7 +859,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -831,7 +870,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -842,7 +881,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -853,7 +892,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -864,7 +903,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -875,7 +914,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -886,7 +925,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -897,7 +936,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -908,7 +947,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -919,7 +958,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -930,7 +969,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -941,7 +980,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -952,7 +991,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -963,7 +1002,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -974,7 +1013,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -985,7 +1024,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -996,7 +1035,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1007,7 +1046,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1018,7 +1057,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1029,7 +1068,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1040,7 +1079,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1068,6 +1107,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006C266C02A97D1D41B60FC5BB4AB3B561" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4b12e3bfb62cc8e0d480f11bb3af7cc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3c01d95-e195-4940-9fb4-afa395d98e0b" xmlns:ns3="77012c7d-7b27-41e5-8843-0f8877a4d830" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f0b17c4e0e330c3092c651d54c7b73f6" ns2:_="" ns3:_="">
     <xsd:import namespace="f3c01d95-e195-4940-9fb4-afa395d98e0b"/>
@@ -1296,23 +1344,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D4A81F4-5E92-4982-94A8-3E41867A3206}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D4A81F4-5E92-4982-94A8-3E41867A3206}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f3c01d95-e195-4940-9fb4-afa395d98e0b"/>
+    <ds:schemaRef ds:uri="77012c7d-7b27-41e5-8843-0f8877a4d830"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C3B8D18-FD30-4E52-B3E9-88E97178C3DC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26A130F8-7154-4D3F-86F2-4BE6BC8F29A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26A130F8-7154-4D3F-86F2-4BE6BC8F29A8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C3B8D18-FD30-4E52-B3E9-88E97178C3DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f3c01d95-e195-4940-9fb4-afa395d98e0b"/>
+    <ds:schemaRef ds:uri="77012c7d-7b27-41e5-8843-0f8877a4d830"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>